<commit_message>
Customer add and delete function, including unit tests
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/12_only_2_customer_care_agents.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/12_only_2_customer_care_agents.xlsx
@@ -177,10 +177,10 @@
   <dimension ref="B1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>

</xml_diff>